<commit_message>
all project changeed.add log model
</commit_message>
<xml_diff>
--- a/TestInterface/InterfaceSuits/测试用例.xlsx
+++ b/TestInterface/InterfaceSuits/测试用例.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,22 +38,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>请求报文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回报文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>请求头</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中天不动产登记平台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,18 +50,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>对外查询接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>预期结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/service-bizz/fj/getDaglHxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>所属模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,107 +62,112 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>根据ID获取有效的申请信息子表数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/service-bizz/YW02/getBdcdyxxById</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID=103610642582</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID=200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据ID查找安置清单表信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/service-bizz/ywbd/azqd/getAzqdById</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询服务器时间（未知参数）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/service-bizz/ywbd/azqd/getFwqsj</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登记平台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/service-core/YW01/getCfQlrxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询查封权利人信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>post</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"Content-Type":"application/x-www-form-urlencoded"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"bdcdyh":"320282999999GB99999F00004049"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getDaglHxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getCfQlrxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getBdcdyxxById</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getAzqdById</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getFwqsj</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>接口标识</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test_getDaglHxx001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_getBdcdyxxById001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_getAzqdById001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_getFwqsj001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_getCfQlrxx001</t>
+    <t>tdcx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对外查询接口(土地信息)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dycx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_getDyxx001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对外查询接口(抵押信息)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/out/isaip/tdcx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"ZDDM":"321202406206GB00169"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Content-Type":"application/json"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/out/isaip/dycx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"BDCZMH":"泰州他项(2012)第7118号"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygcx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_getYgxx001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/out/isaip/ygcx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_getYgxx002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对外查询接口(预告、预抵押、预查封信息)（商品房）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对外查询接口(预告、预抵押、预查封信息)（存量房）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{"FWDM": "FHID800020469"}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"BDCDYH": "",
+"FWDM": "",
+"FWZL": "",
+"YGQLR": "",
+"YGZMH": "苏(2019)泰州不动产证明第0000510号",
+"ZJHM": ""
+}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_getTdxx001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"城镇住宅用地"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"泰州国用(2012)第10424号"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"苏(2019)泰州不动产证明第0000510号"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"苏（2020）宜兴不动产证明第0008948号"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -262,16 +247,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -281,10 +263,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,10 +565,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -594,207 +576,181 @@
     <col min="1" max="1" width="17.75" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="33.625" customWidth="1"/>
-    <col min="7" max="7" width="55.875" customWidth="1"/>
-    <col min="8" max="8" width="60" customWidth="1"/>
+    <col min="5" max="5" width="44.875" customWidth="1"/>
+    <col min="7" max="7" width="20.25" customWidth="1"/>
+    <col min="8" max="8" width="37.5" customWidth="1"/>
     <col min="9" max="9" width="48" customWidth="1"/>
-    <col min="12" max="12" width="26.375" customWidth="1"/>
+    <col min="10" max="10" width="47.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="121.5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>12</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="78" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="4"/>
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="H8" s="5"/>
+    <row r="6" spans="1:10">
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="http://172.0.0.103:1100/service-bizz/fj/getDaglHxx"/>
-    <hyperlink ref="G4" r:id="rId2" display="http://172.0.0.103:1100/service-bizz/ywbd/azqd/getAzqdById"/>
+    <hyperlink ref="G4" r:id="rId1" display="http://172.0.0.103:1100/service-bizz/ywbd/azqd/getAzqdById"/>
+    <hyperlink ref="G5" r:id="rId2" display="http://172.0.0.103:1100/service-bizz/ywbd/azqd/getAzqdById"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
@@ -821,7 +777,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>

</xml_diff>